<commit_message>
Test-4 for hybrid model (synth classification)
</commit_message>
<xml_diff>
--- a/migforecasting/Hybridization/exp/test-4.xlsx
+++ b/migforecasting/Hybridization/exp/test-4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="10">
   <si>
     <t>test input (MAPE)</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>test input (MAE)</t>
+  </si>
+  <si>
+    <t>Hybrid model-KZ (citiesdataset-NYDcor-4.csv) - non-synth</t>
+  </si>
+  <si>
+    <t>Hybrid model-KZ (citiesdataset-NYDcor-4.csv) - synth</t>
   </si>
 </sst>
 </file>
@@ -388,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AD108"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH97" sqref="AH97"/>
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH84" sqref="AH84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4955,14 +4961,2399 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C3:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U66" sqref="U66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>631.93844448889297</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>430.07272069188872</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>556.93590572255846</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>612.8443823103587</v>
+      </c>
+      <c r="I7" s="2">
+        <f>I6+1</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>423.03665528441309</v>
+      </c>
+      <c r="N7" s="2">
+        <f>N6+1</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="3">
+        <v>517.41628490875109</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C71" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>683.37854216672315</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" ref="I8:I71" si="1">I7+1</f>
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>455.9829391930507</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" ref="N8:N71" si="2">N7+1</f>
+        <v>3</v>
+      </c>
+      <c r="O8" s="3">
+        <v>461.58674253247949</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>615.4559013887291</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J9" s="3">
+        <v>352.04807644683189</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O9" s="3">
+        <v>548.57339300681974</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>661.57610055434793</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J10" s="3">
+        <v>377.92065174115118</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O10" s="3">
+        <v>483.42449879986259</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>674.47370728083115</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J11" s="3">
+        <v>444.23433120928081</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O11" s="3">
+        <v>462.79265158875268</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>548.23537685259168</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J12" s="3">
+        <v>411.66427506000662</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O12" s="3">
+        <v>518.57942088619609</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>704.68394335543019</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J13" s="3">
+        <v>466.10909584904948</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O13" s="3">
+        <v>544.62248714138741</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>702.90565931344474</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J14" s="3">
+        <v>417.29583419057411</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O14" s="3">
+        <v>461.19460576446829</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>615.05605569207842</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J15" s="3">
+        <v>480.8304350020951</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O15" s="3">
+        <v>508.33934678248909</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>667.37086333676154</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J16" s="3">
+        <v>429.40552429801511</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O16" s="3">
+        <v>512.11807678020307</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>707.06897983578995</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J17" s="3">
+        <v>487.59229073798889</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O17" s="3">
+        <v>447.42857717072388</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>663.1831702194529</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J18" s="3">
+        <v>408.51169571760539</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O18" s="3">
+        <v>621.52393111593642</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>586.4359219148846</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J19" s="3">
+        <v>517.7840792281022</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O19" s="3">
+        <v>523.41101687811897</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>564.20895621404247</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J20" s="3">
+        <v>411.29543357336041</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O20" s="3">
+        <v>445.88829899607498</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>680.89242689640605</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J21" s="3">
+        <v>445.65006605516771</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O21" s="3">
+        <v>518.00896526269628</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>673.85630524440819</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J22" s="3">
+        <v>436.699919419362</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O22" s="3">
+        <v>450.12622352078301</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>626.86025826761067</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J23" s="3">
+        <v>453.12367689640689</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O23" s="3">
+        <v>551.38458199984723</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>571.7426509220096</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J24" s="3">
+        <v>505.53328494685059</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O24" s="3">
+        <v>541.11366389492105</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>707.61095406141555</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J25" s="3">
+        <v>425.06780070103241</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O25" s="3">
+        <v>534.62636148893159</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>615.81746866308413</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J26" s="3">
+        <v>444.98870609021958</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O26" s="3">
+        <v>434.72494251723958</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>539.00364303539368</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J27" s="3">
+        <v>409.08719415552241</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O27" s="3">
+        <v>465.42379957709409</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="3">
+        <v>545.24698970358429</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J28" s="3">
+        <v>445.23738384386752</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O28" s="3">
+        <v>497.40902322170132</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="3">
+        <v>640.4768687373786</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J29" s="3">
+        <v>449.38442517240043</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O29" s="3">
+        <v>461.07035956490262</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>576.90834871604272</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J30" s="3">
+        <v>457.84652588867249</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O30" s="3">
+        <v>419.767842658208</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>526.46703308949532</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J31" s="3">
+        <v>436.91184621099552</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O31" s="3">
+        <v>518.64386167942985</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>448.36962700499021</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J32" s="3">
+        <v>458.51934840172191</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O32" s="3">
+        <v>521.02554934849672</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="3">
+        <v>640.06556949365552</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J33" s="3">
+        <v>520.59907341791416</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O33" s="3">
+        <v>418.35238779670021</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>670.04271873928337</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J34" s="3">
+        <v>434.14997275879142</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O34" s="3">
+        <v>494.68877209776338</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
+        <v>695.16442145768951</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J35" s="3">
+        <v>495.7654067131478</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O35" s="3">
+        <v>504.70239108279031</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="3">
+        <v>715.15056811254533</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J36" s="3">
+        <v>462.59606035927891</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O36" s="3">
+        <v>554.27898445536596</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>720.64686954699471</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J37" s="3">
+        <v>387.56195408046591</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O37" s="3">
+        <v>505.60062197584477</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
+        <v>589.09323389339681</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J38" s="3">
+        <v>471.43802282165569</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O38" s="3">
+        <v>515.51553153693749</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="3">
+        <v>657.32607921857652</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J39" s="3">
+        <v>419.51543485922173</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O39" s="3">
+        <v>422.46836190802719</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>679.52828809006655</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J40" s="3">
+        <v>414.35183478111782</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O40" s="3">
+        <v>569.41701689716888</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="3">
+        <v>672.79925077151586</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J41" s="3">
+        <v>402.03200761039352</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O41" s="3">
+        <v>528.04636229854827</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="3">
+        <v>702.60497947384385</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J42" s="3">
+        <v>426.93381662666189</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O42" s="3">
+        <v>527.32177815559862</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="3">
+        <v>737.14053301329591</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J43" s="3">
+        <v>369.06831185468792</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O43" s="3">
+        <v>444.01380567302903</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>595.72421952985007</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J44" s="3">
+        <v>431.40742508667631</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O44" s="3">
+        <v>543.86772459709675</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3">
+        <v>716.15331204518498</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J45" s="3">
+        <v>502.96395973825571</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O45" s="3">
+        <v>502.10623690326491</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3">
+        <v>712.97552244065912</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J46" s="3">
+        <v>414.90330237741432</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O46" s="3">
+        <v>543.67853916638057</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="3">
+        <v>671.85655160589704</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J47" s="3">
+        <v>429.61061206995049</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O47" s="3">
+        <v>535.72977592677239</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="3">
+        <v>719.6615732274156</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J48" s="3">
+        <v>478.43329323351202</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O48" s="3">
+        <v>636.31500038099557</v>
+      </c>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>701.4176171086209</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J49" s="3">
+        <v>411.96718358288558</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O49" s="3">
+        <v>463.35596730102452</v>
+      </c>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="3">
+        <v>627.54524945707999</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J50" s="3">
+        <v>469.38355874004611</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O50" s="3">
+        <v>462.74279641482798</v>
+      </c>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3">
+        <v>643.0341393302084</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J51" s="3">
+        <v>513.41369189812167</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O51" s="3">
+        <v>459.3859027698399</v>
+      </c>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="3">
+        <v>724.04721396730963</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J52" s="3">
+        <v>418.29663947308211</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O52" s="3">
+        <v>462.87132767554323</v>
+      </c>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="3">
+        <v>655.69785208785709</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J53" s="3">
+        <v>451.71894645102282</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O53" s="3">
+        <v>419.55648240751282</v>
+      </c>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3">
+        <v>732.12783279993823</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J54" s="3">
+        <v>484.3316855735892</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O54" s="3">
+        <v>516.82326537318534</v>
+      </c>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="3">
+        <v>698.64593586886031</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J55" s="3">
+        <v>371.49122628300358</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O55" s="3">
+        <v>473.80054777688821</v>
+      </c>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="D56" s="3">
+        <v>662.82366846687148</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="J56" s="3">
+        <v>541.3013684421071</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="O56" s="3">
+        <v>554.24581742675332</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="2">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D57" s="3">
+        <v>709.59265497009085</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="J57" s="3">
+        <v>555.88025979159499</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="O57" s="3">
+        <v>494.97552067855349</v>
+      </c>
+    </row>
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C58" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="D58" s="3">
+        <v>591.93472854040363</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="J58" s="3">
+        <v>519.96773759858206</v>
+      </c>
+      <c r="N58" s="2">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="O58" s="3">
+        <v>429.32259277250711</v>
+      </c>
+    </row>
+    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C59" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="D59" s="3">
+        <v>683.00254490989346</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="J59" s="3">
+        <v>553.28334257248389</v>
+      </c>
+      <c r="N59" s="2">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="O59" s="3">
+        <v>474.82154189050152</v>
+      </c>
+    </row>
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C60" s="2">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="D60" s="3">
+        <v>605.76398159789608</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="J60" s="3">
+        <v>529.50752271688145</v>
+      </c>
+      <c r="N60" s="2">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="O60" s="3">
+        <v>358.30765511296482</v>
+      </c>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C61" s="2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D61" s="3">
+        <v>631.61605335847833</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="J61" s="3">
+        <v>603.23190988493855</v>
+      </c>
+      <c r="N61" s="2">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="O61" s="3">
+        <v>504.3761660380232</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C62" s="2">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D62" s="3">
+        <v>536.89878243227713</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="J62" s="3">
+        <v>549.46397821655762</v>
+      </c>
+      <c r="N62" s="2">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="O62" s="3">
+        <v>536.34678534689658</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C63" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="D63" s="3">
+        <v>719.67908646702381</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="J63" s="3">
+        <v>485.03854211909868</v>
+      </c>
+      <c r="N63" s="2">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="O63" s="3">
+        <v>443.62140058863849</v>
+      </c>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C64" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="D64" s="3">
+        <v>700.70023840819795</v>
+      </c>
+      <c r="I64" s="2">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="J64" s="3">
+        <v>510.47556273097831</v>
+      </c>
+      <c r="N64" s="2">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="O64" s="3">
+        <v>533.25201199184619</v>
+      </c>
+    </row>
+    <row r="65" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C65" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D65" s="3">
+        <v>547.31272288261414</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J65" s="3">
+        <v>493.64634729683348</v>
+      </c>
+      <c r="N65" s="2">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="O65" s="3">
+        <v>490.8228805673026</v>
+      </c>
+    </row>
+    <row r="66" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C66" s="2">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D66" s="3">
+        <v>592.0511680858757</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="J66" s="3">
+        <v>518.35575065721764</v>
+      </c>
+      <c r="N66" s="2">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="O66" s="3">
+        <v>552.96093339238735</v>
+      </c>
+    </row>
+    <row r="67" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C67" s="2">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="D67" s="3">
+        <v>643.89814231150137</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="J67" s="3">
+        <v>516.66748137882371</v>
+      </c>
+      <c r="N67" s="2">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="O67" s="3">
+        <v>508.43613798719798</v>
+      </c>
+    </row>
+    <row r="68" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C68" s="2">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="D68" s="3">
+        <v>682.54901698289234</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="J68" s="3">
+        <v>490.41117246732921</v>
+      </c>
+      <c r="N68" s="2">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="O68" s="3">
+        <v>504.69717443898332</v>
+      </c>
+    </row>
+    <row r="69" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C69" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D69" s="3">
+        <v>697.01019206956903</v>
+      </c>
+      <c r="I69" s="2">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="J69" s="3">
+        <v>558.10026755438662</v>
+      </c>
+      <c r="N69" s="2">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="O69" s="3">
+        <v>463.48680153922322</v>
+      </c>
+    </row>
+    <row r="70" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C70" s="2">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="D70" s="3">
+        <v>628.49063954928124</v>
+      </c>
+      <c r="I70" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="J70" s="3">
+        <v>456.47044252676432</v>
+      </c>
+      <c r="N70" s="2">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="O70" s="3">
+        <v>547.34975706747412</v>
+      </c>
+    </row>
+    <row r="71" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C71" s="2">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="D71" s="3">
+        <v>637.42032913285209</v>
+      </c>
+      <c r="I71" s="2">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="J71" s="3">
+        <v>484.83592410561153</v>
+      </c>
+      <c r="N71" s="2">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="O71" s="3">
+        <v>423.69179253819448</v>
+      </c>
+    </row>
+    <row r="72" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C72" s="2">
+        <f t="shared" ref="C72:C105" si="3">C71+1</f>
+        <v>67</v>
+      </c>
+      <c r="D72" s="3">
+        <v>589.13995828094539</v>
+      </c>
+      <c r="I72" s="2">
+        <f t="shared" ref="I72:I105" si="4">I71+1</f>
+        <v>67</v>
+      </c>
+      <c r="J72" s="3">
+        <v>525.48951418257275</v>
+      </c>
+      <c r="N72" s="2">
+        <f t="shared" ref="N72:N105" si="5">N71+1</f>
+        <v>67</v>
+      </c>
+      <c r="O72" s="3">
+        <v>463.33935044957491</v>
+      </c>
+    </row>
+    <row r="73" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C73" s="2">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="D73" s="3">
+        <v>608.07559973520711</v>
+      </c>
+      <c r="I73" s="2">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="J73" s="3">
+        <v>450.73154360498302</v>
+      </c>
+      <c r="N73" s="2">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="O73" s="3">
+        <v>492.83281379776707</v>
+      </c>
+    </row>
+    <row r="74" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C74" s="2">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="D74" s="3">
+        <v>670.91919252676416</v>
+      </c>
+      <c r="I74" s="2">
+        <f t="shared" si="4"/>
+        <v>69</v>
+      </c>
+      <c r="J74" s="3">
+        <v>501.19451194422157</v>
+      </c>
+      <c r="N74" s="2">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="O74" s="3">
+        <v>493.21154989141581</v>
+      </c>
+    </row>
+    <row r="75" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C75" s="2">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="D75" s="3">
+        <v>584.93805106297748</v>
+      </c>
+      <c r="I75" s="2">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="J75" s="3">
+        <v>524.52931554082295</v>
+      </c>
+      <c r="N75" s="2">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="O75" s="3">
+        <v>450.48990289366338</v>
+      </c>
+    </row>
+    <row r="76" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C76" s="2">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="D76" s="3">
+        <v>674.22932887568015</v>
+      </c>
+      <c r="I76" s="2">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="J76" s="3">
+        <v>559.26159442031428</v>
+      </c>
+      <c r="N76" s="2">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="O76" s="3">
+        <v>471.18343548786498</v>
+      </c>
+    </row>
+    <row r="77" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C77" s="2">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="D77" s="3">
+        <v>740.34852649826553</v>
+      </c>
+      <c r="I77" s="2">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="J77" s="3">
+        <v>495.8107172248254</v>
+      </c>
+      <c r="N77" s="2">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="O77" s="3">
+        <v>586.87907994246916</v>
+      </c>
+    </row>
+    <row r="78" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C78" s="2">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="D78" s="3">
+        <v>645.35519778450782</v>
+      </c>
+      <c r="I78" s="2">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+      <c r="J78" s="3">
+        <v>577.76400550539063</v>
+      </c>
+      <c r="N78" s="2">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="O78" s="3">
+        <v>477.58249476130578</v>
+      </c>
+    </row>
+    <row r="79" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C79" s="2">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="D79" s="3">
+        <v>557.92731288337632</v>
+      </c>
+      <c r="I79" s="2">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
+      <c r="J79" s="3">
+        <v>500.11302801272478</v>
+      </c>
+      <c r="N79" s="2">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="O79" s="3">
+        <v>526.80959700156188</v>
+      </c>
+    </row>
+    <row r="80" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C80" s="2">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="D80" s="3">
+        <v>595.21362665256879</v>
+      </c>
+      <c r="I80" s="2">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="J80" s="3">
+        <v>494.69918119213571</v>
+      </c>
+      <c r="N80" s="2">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="O80" s="3">
+        <v>464.42791347582568</v>
+      </c>
+    </row>
+    <row r="81" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C81" s="2">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="D81" s="3">
+        <v>693.94877876519138</v>
+      </c>
+      <c r="I81" s="2">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="J81" s="3">
+        <v>452.4043613079586</v>
+      </c>
+      <c r="N81" s="2">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="O81" s="3">
+        <v>594.13315026479165</v>
+      </c>
+    </row>
+    <row r="82" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C82" s="2">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="D82" s="3">
+        <v>619.53063816817064</v>
+      </c>
+      <c r="I82" s="2">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="J82" s="3">
+        <v>515.7476279670052</v>
+      </c>
+      <c r="N82" s="2">
+        <f t="shared" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="O82" s="3">
+        <v>575.46546005257721</v>
+      </c>
+    </row>
+    <row r="83" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C83" s="2">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="D83" s="3">
+        <v>745.39912637634677</v>
+      </c>
+      <c r="I83" s="2">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+      <c r="J83" s="3">
+        <v>548.08882329409028</v>
+      </c>
+      <c r="N83" s="2">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="O83" s="3">
+        <v>409.48624919038332</v>
+      </c>
+    </row>
+    <row r="84" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C84" s="2">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="D84" s="3">
+        <v>664.9532364174944</v>
+      </c>
+      <c r="I84" s="2">
+        <f t="shared" si="4"/>
+        <v>79</v>
+      </c>
+      <c r="J84" s="3">
+        <v>473.13686087933809</v>
+      </c>
+      <c r="N84" s="2">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="O84" s="3">
+        <v>486.55303439440638</v>
+      </c>
+    </row>
+    <row r="85" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C85" s="2">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="D85" s="3">
+        <v>727.83003405150953</v>
+      </c>
+      <c r="I85" s="2">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="J85" s="3">
+        <v>476.08216586657471</v>
+      </c>
+      <c r="N85" s="2">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="O85" s="3">
+        <v>499.88067536289827</v>
+      </c>
+    </row>
+    <row r="86" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C86" s="2">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="D86" s="3">
+        <v>706.24545924296035</v>
+      </c>
+      <c r="I86" s="2">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="J86" s="3">
+        <v>519.87633943879246</v>
+      </c>
+      <c r="N86" s="2">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="O86" s="3">
+        <v>480.21904222387298</v>
+      </c>
+    </row>
+    <row r="87" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C87" s="2">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="D87" s="3">
+        <v>637.22879967234269</v>
+      </c>
+      <c r="I87" s="2">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+      <c r="J87" s="3">
+        <v>542.46205990208352</v>
+      </c>
+      <c r="N87" s="2">
+        <f t="shared" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="O87" s="3">
+        <v>466.37646340534133</v>
+      </c>
+    </row>
+    <row r="88" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C88" s="2">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="D88" s="3">
+        <v>564.86507819941232</v>
+      </c>
+      <c r="I88" s="2">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+      <c r="J88" s="3">
+        <v>605.13051567798175</v>
+      </c>
+      <c r="N88" s="2">
+        <f t="shared" si="5"/>
+        <v>83</v>
+      </c>
+      <c r="O88" s="3">
+        <v>484.96040014096849</v>
+      </c>
+    </row>
+    <row r="89" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C89" s="2">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="D89" s="3">
+        <v>598.86244851792503</v>
+      </c>
+      <c r="I89" s="2">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="J89" s="3">
+        <v>504.02146469120243</v>
+      </c>
+      <c r="N89" s="2">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="O89" s="3">
+        <v>470.74984288680582</v>
+      </c>
+    </row>
+    <row r="90" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C90" s="2">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="D90" s="3">
+        <v>634.57525712462291</v>
+      </c>
+      <c r="I90" s="2">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="J90" s="3">
+        <v>486.71882262734738</v>
+      </c>
+      <c r="N90" s="2">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="O90" s="3">
+        <v>481.6046542938235</v>
+      </c>
+    </row>
+    <row r="91" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C91" s="2">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="D91" s="3">
+        <v>705.25006462643273</v>
+      </c>
+      <c r="I91" s="2">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="J91" s="3">
+        <v>562.87317917285736</v>
+      </c>
+      <c r="N91" s="2">
+        <f t="shared" si="5"/>
+        <v>86</v>
+      </c>
+      <c r="O91" s="3">
+        <v>506.61303368003968</v>
+      </c>
+    </row>
+    <row r="92" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C92" s="2">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="D92" s="3">
+        <v>696.28970420428925</v>
+      </c>
+      <c r="I92" s="2">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="J92" s="3">
+        <v>502.90693326856382</v>
+      </c>
+      <c r="N92" s="2">
+        <f t="shared" si="5"/>
+        <v>87</v>
+      </c>
+      <c r="O92" s="3">
+        <v>571.30989084466762</v>
+      </c>
+    </row>
+    <row r="93" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C93" s="2">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="D93" s="3">
+        <v>642.07998118832541</v>
+      </c>
+      <c r="I93" s="2">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="J93" s="3">
+        <v>477.87803487065128</v>
+      </c>
+      <c r="N93" s="2">
+        <f t="shared" si="5"/>
+        <v>88</v>
+      </c>
+      <c r="O93" s="3">
+        <v>464.72972849277983</v>
+      </c>
+    </row>
+    <row r="94" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C94" s="2">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="D94" s="3">
+        <v>574.08363241513234</v>
+      </c>
+      <c r="I94" s="2">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+      <c r="J94" s="3">
+        <v>515.05813188173818</v>
+      </c>
+      <c r="N94" s="2">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="O94" s="3">
+        <v>524.95456733150445</v>
+      </c>
+    </row>
+    <row r="95" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C95" s="2">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="D95" s="3">
+        <v>633.42607550386617</v>
+      </c>
+      <c r="I95" s="2">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="J95" s="3">
+        <v>550.40638692040943</v>
+      </c>
+      <c r="N95" s="2">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="O95" s="3">
+        <v>462.2807428944256</v>
+      </c>
+    </row>
+    <row r="96" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C96" s="2">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="D96" s="3">
+        <v>655.94014392120914</v>
+      </c>
+      <c r="I96" s="2">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="J96" s="3">
+        <v>494.08229345258479</v>
+      </c>
+      <c r="N96" s="2">
+        <f t="shared" si="5"/>
+        <v>91</v>
+      </c>
+      <c r="O96" s="3">
+        <v>484.43005333942921</v>
+      </c>
+    </row>
+    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C97" s="2">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="D97" s="3">
+        <v>565.92207042709549</v>
+      </c>
+      <c r="I97" s="2">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="J97" s="3">
+        <v>551.94372714024428</v>
+      </c>
+      <c r="N97" s="2">
+        <f t="shared" si="5"/>
+        <v>92</v>
+      </c>
+      <c r="O97" s="3">
+        <v>499.5211912790034</v>
+      </c>
+    </row>
+    <row r="98" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C98" s="2">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="D98" s="3">
+        <v>628.42863051015263</v>
+      </c>
+      <c r="I98" s="2">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="J98" s="3">
+        <v>585.07019845125114</v>
+      </c>
+      <c r="N98" s="2">
+        <f t="shared" si="5"/>
+        <v>93</v>
+      </c>
+      <c r="O98" s="3">
+        <v>450.27558678134608</v>
+      </c>
+    </row>
+    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C99" s="2">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="D99" s="3">
+        <v>735.03061635615404</v>
+      </c>
+      <c r="I99" s="2">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="J99" s="3">
+        <v>533.11944274583709</v>
+      </c>
+      <c r="N99" s="2">
+        <f t="shared" si="5"/>
+        <v>94</v>
+      </c>
+      <c r="O99" s="3">
+        <v>476.7264226864022</v>
+      </c>
+    </row>
+    <row r="100" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C100" s="2">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="D100" s="3">
+        <v>702.47361684192379</v>
+      </c>
+      <c r="I100" s="2">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="J100" s="3">
+        <v>506.24124047510139</v>
+      </c>
+      <c r="N100" s="2">
+        <f t="shared" si="5"/>
+        <v>95</v>
+      </c>
+      <c r="O100" s="3">
+        <v>548.12038080542493</v>
+      </c>
+    </row>
+    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C101" s="2">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="D101" s="3">
+        <v>584.02369013601469</v>
+      </c>
+      <c r="I101" s="2">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="J101" s="3">
+        <v>551.82447141578041</v>
+      </c>
+      <c r="N101" s="2">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
+      <c r="O101" s="3">
+        <v>527.93950370518496</v>
+      </c>
+    </row>
+    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C102" s="2">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="D102" s="3">
+        <v>631.75472358745674</v>
+      </c>
+      <c r="I102" s="2">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="J102" s="3">
+        <v>479.54984722063432</v>
+      </c>
+      <c r="N102" s="2">
+        <f t="shared" si="5"/>
+        <v>97</v>
+      </c>
+      <c r="O102" s="3">
+        <v>480.19569436506993</v>
+      </c>
+    </row>
+    <row r="103" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C103" s="2">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="D103" s="3">
+        <v>673.91372099668456</v>
+      </c>
+      <c r="I103" s="2">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="J103" s="3">
+        <v>531.38712267116205</v>
+      </c>
+      <c r="N103" s="2">
+        <f t="shared" si="5"/>
+        <v>98</v>
+      </c>
+      <c r="O103" s="3">
+        <v>454.12414328304129</v>
+      </c>
+    </row>
+    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C104" s="2">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="D104" s="3">
+        <v>607.50250352421142</v>
+      </c>
+      <c r="I104" s="2">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="J104" s="3">
+        <v>605.74414214005378</v>
+      </c>
+      <c r="N104" s="2">
+        <f t="shared" si="5"/>
+        <v>99</v>
+      </c>
+      <c r="O104" s="3">
+        <v>505.26222030136722</v>
+      </c>
+    </row>
+    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C105" s="2">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="D105" s="3">
+        <v>720.46328075589508</v>
+      </c>
+      <c r="I105" s="2">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="J105" s="3">
+        <v>504.18398812245169</v>
+      </c>
+      <c r="N105" s="2">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="O105" s="3">
+        <v>532.17325241932383</v>
+      </c>
+    </row>
+    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107" s="3">
+        <f>AVERAGE(D6:D105)</f>
+        <v>647.57430166542758</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J107" s="3">
+        <f>AVERAGE(J6:J105)</f>
+        <v>481.359368396864</v>
+      </c>
+      <c r="N107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O107" s="3">
+        <f>AVERAGE(O6:O105)</f>
+        <v>497.17356484883953</v>
+      </c>
+    </row>
+    <row r="108" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="3">
+        <f>_xlfn.STDEV.S(D6:D105)</f>
+        <v>59.216547487236269</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J108" s="3">
+        <f>_xlfn.STDEV.S(J6:J105)</f>
+        <v>55.733006534081184</v>
+      </c>
+      <c r="N108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O108" s="3">
+        <f>_xlfn.STDEV.S(O6:O105)</f>
+        <v>47.547921354532939</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>